<commit_message>
testing results file updated
</commit_message>
<xml_diff>
--- a/Docs/log_debug9Sep2016.xlsx
+++ b/Docs/log_debug9Sep2016.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\projects\sequential_invest\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\projects\sequential_invest\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="9-10Sep2016" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="14">
   <si>
     <t>k</t>
   </si>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -273,44 +273,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>578909</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>164042</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>63500</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>102037</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4494742" y="5498042"/>
-          <a:ext cx="5009091" cy="2604995"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
       <xdr:col>17</xdr:col>
       <xdr:colOff>31750</xdr:colOff>
       <xdr:row>13</xdr:row>
@@ -330,7 +292,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -368,7 +330,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -406,7 +368,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -415,6 +377,82 @@
         <a:xfrm>
           <a:off x="16531167" y="4550835"/>
           <a:ext cx="4635499" cy="2767576"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>285751</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>113104</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>603250</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>158847</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16520584" y="1637104"/>
+          <a:ext cx="4614333" cy="2903243"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>603250</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>21167</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>21167</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>82833</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4519083" y="5545667"/>
+          <a:ext cx="4942417" cy="3109666"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -725,8 +763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1222,7 +1260,12 @@
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
-      <c r="P18" s="2"/>
+      <c r="P18" s="4">
+        <v>-0.125</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
@@ -1458,7 +1501,9 @@
       <c r="D31" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E31" s="4"/>
+      <c r="E31" s="4">
+        <v>1E-3</v>
+      </c>
       <c r="F31" s="6" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
remove market from choice, add single stock test
</commit_message>
<xml_diff>
--- a/Docs/log_debug9Sep2016.xlsx
+++ b/Docs/log_debug9Sep2016.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="9-10Sep2016" sheetId="1" r:id="rId1"/>
+    <sheet name="11Sep2016" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -464,6 +465,353 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>346075</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="76200"/>
+          <a:ext cx="5222875" cy="3286125"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>171451</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>391493</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>57151</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1" y="3409951"/>
+          <a:ext cx="5268292" cy="3314700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>400051</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>495301</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>80311</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5276851" y="3429000"/>
+          <a:ext cx="4972050" cy="3128311"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>556847</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>582492</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>175165</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5421924" y="0"/>
+          <a:ext cx="5498856" cy="3413665"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>326671</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>171451</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>413921</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>57151</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10664959" y="361951"/>
+          <a:ext cx="4952327" cy="3124200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>73269</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>146537</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>600608</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>87922</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15884769" y="146537"/>
+          <a:ext cx="4784281" cy="3179885"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>153865</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>487185</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>2929</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15965365" y="3429000"/>
+          <a:ext cx="4590262" cy="3050929"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>564172</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>194107</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>130121</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20632614" y="190500"/>
+          <a:ext cx="4495012" cy="2987621"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>520212</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>161193</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>127635</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20588654" y="3209193"/>
+          <a:ext cx="4535365" cy="3014442"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -763,7 +1111,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
@@ -1581,4 +1929,19 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="AC7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AQ30" sqref="AQ30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
log of tests with knee classifier
</commit_message>
<xml_diff>
--- a/Docs/log_debug9Sep2016.xlsx
+++ b/Docs/log_debug9Sep2016.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="9-10Sep2016" sheetId="1" r:id="rId1"/>
     <sheet name="11Sep2016" sheetId="2" r:id="rId2"/>
+    <sheet name="13Sep2016" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="17">
   <si>
     <t>k</t>
   </si>
@@ -68,12 +69,21 @@
   <si>
     <t>-------------------------------------------------------------------------------------------------------------------------------------&gt;</t>
   </si>
+  <si>
+    <t>2008/7/20 - 2009/1/20</t>
+  </si>
+  <si>
+    <t>optimize_l</t>
+  </si>
+  <si>
+    <t>limited stocks</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,13 +91,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -154,7 +184,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -164,6 +194,10 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -173,6 +207,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1111,8 +1156,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q33"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1155,10 +1200,10 @@
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="9">
         <v>10</v>
       </c>
       <c r="C2" s="3">
@@ -1185,8 +1230,8 @@
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
       <c r="C3" s="3">
         <v>0</v>
       </c>
@@ -1211,8 +1256,8 @@
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="10"/>
       <c r="C4" s="3">
         <v>20</v>
       </c>
@@ -1237,8 +1282,8 @@
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="9"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="11"/>
       <c r="C5" s="3">
         <v>20</v>
       </c>
@@ -1263,8 +1308,8 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="7">
+      <c r="A6" s="10"/>
+      <c r="B6" s="9">
         <v>5</v>
       </c>
       <c r="C6" s="3">
@@ -1291,8 +1336,8 @@
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
       <c r="C7" s="3">
         <v>0</v>
       </c>
@@ -1317,8 +1362,8 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
       <c r="C8" s="3">
         <v>20</v>
       </c>
@@ -1343,8 +1388,8 @@
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="9"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="11"/>
       <c r="C9" s="3">
         <v>20</v>
       </c>
@@ -1369,8 +1414,8 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="7" t="s">
+      <c r="A10" s="10"/>
+      <c r="B10" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="3">
@@ -1397,8 +1442,8 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
       <c r="C11" s="3">
         <v>0</v>
       </c>
@@ -1423,8 +1468,8 @@
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
+      <c r="A12" s="10"/>
+      <c r="B12" s="10"/>
       <c r="C12" s="3">
         <v>20</v>
       </c>
@@ -1449,8 +1494,8 @@
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="9"/>
+      <c r="A13" s="10"/>
+      <c r="B13" s="11"/>
       <c r="C13" s="3">
         <v>20</v>
       </c>
@@ -1475,8 +1520,8 @@
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="7" t="s">
+      <c r="A14" s="10"/>
+      <c r="B14" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="3">
@@ -1503,8 +1548,8 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
       <c r="C15" s="3">
         <v>0</v>
       </c>
@@ -1529,8 +1574,8 @@
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
       <c r="C16" s="3">
         <v>20</v>
       </c>
@@ -1555,8 +1600,8 @@
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
-      <c r="B17" s="9"/>
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
       <c r="C17" s="3">
         <v>20</v>
       </c>
@@ -1581,10 +1626,10 @@
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C18" s="3">
@@ -1616,8 +1661,8 @@
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
+      <c r="A19" s="10"/>
+      <c r="B19" s="10"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="2"/>
@@ -1634,8 +1679,8 @@
       <c r="P19" s="2"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
+      <c r="A20" s="10"/>
+      <c r="B20" s="10"/>
       <c r="C20" s="3">
         <v>20</v>
       </c>
@@ -1661,8 +1706,8 @@
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
+      <c r="A21" s="10"/>
+      <c r="B21" s="10"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="2"/>
@@ -1679,8 +1724,8 @@
       <c r="P21" s="2"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
+      <c r="A22" s="10"/>
+      <c r="B22" s="10"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="2"/>
@@ -1697,8 +1742,8 @@
       <c r="P22" s="2"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8"/>
+      <c r="A23" s="10"/>
+      <c r="B23" s="10"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="2"/>
@@ -1715,8 +1760,8 @@
       <c r="P23" s="2"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
+      <c r="A24" s="10"/>
+      <c r="B24" s="10"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="2"/>
@@ -1733,8 +1778,8 @@
       <c r="P24" s="2"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
-      <c r="B25" s="8"/>
+      <c r="A25" s="10"/>
+      <c r="B25" s="10"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="2"/>
@@ -1751,8 +1796,8 @@
       <c r="P25" s="2"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
+      <c r="A26" s="10"/>
+      <c r="B26" s="10"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="2"/>
@@ -1769,8 +1814,8 @@
       <c r="P26" s="2"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A27" s="8"/>
-      <c r="B27" s="8"/>
+      <c r="A27" s="10"/>
+      <c r="B27" s="10"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="2"/>
@@ -1787,8 +1832,8 @@
       <c r="P27" s="2"/>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A28" s="8"/>
-      <c r="B28" s="8"/>
+      <c r="A28" s="10"/>
+      <c r="B28" s="10"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="2"/>
@@ -1805,8 +1850,8 @@
       <c r="P28" s="2"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A29" s="8"/>
-      <c r="B29" s="8"/>
+      <c r="A29" s="10"/>
+      <c r="B29" s="10"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="2"/>
@@ -1823,8 +1868,8 @@
       <c r="P29" s="2"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A30" s="8"/>
-      <c r="B30" s="8"/>
+      <c r="A30" s="10"/>
+      <c r="B30" s="10"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="2"/>
@@ -1841,8 +1886,8 @@
       <c r="P30" s="2"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A31" s="8"/>
-      <c r="B31" s="8"/>
+      <c r="A31" s="10"/>
+      <c r="B31" s="10"/>
       <c r="C31" s="3">
         <v>0</v>
       </c>
@@ -1872,8 +1917,8 @@
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A32" s="8"/>
-      <c r="B32" s="8"/>
+      <c r="A32" s="10"/>
+      <c r="B32" s="10"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="2"/>
@@ -1890,8 +1935,8 @@
       <c r="P32" s="2"/>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A33" s="9"/>
-      <c r="B33" s="9"/>
+      <c r="A33" s="11"/>
+      <c r="B33" s="11"/>
       <c r="C33" s="3">
         <v>20</v>
       </c>
@@ -1935,7 +1980,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="AD1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="AQ30" sqref="AQ30"/>
     </sheetView>
   </sheetViews>
@@ -1944,4 +1989,293 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="7">
+        <v>10</v>
+      </c>
+      <c r="C2" s="7">
+        <v>20</v>
+      </c>
+      <c r="D2" s="7">
+        <v>0</v>
+      </c>
+      <c r="E2" s="7">
+        <v>0</v>
+      </c>
+      <c r="F2" s="4">
+        <v>-0.52400000000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7">
+        <v>20</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7">
+        <v>1</v>
+      </c>
+      <c r="F3" s="4">
+        <v>5.8000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7">
+        <v>0</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4">
+        <v>-0.38700000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7">
+        <v>0</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7">
+        <v>1</v>
+      </c>
+      <c r="F5" s="4">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="12">
+        <v>20</v>
+      </c>
+      <c r="D6" s="7">
+        <v>0</v>
+      </c>
+      <c r="E6" s="14">
+        <v>1</v>
+      </c>
+      <c r="F6" s="16">
+        <v>0.47299999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="14">
+        <v>20</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7">
+        <v>0</v>
+      </c>
+      <c r="F7" s="4">
+        <v>-0.42299999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="7">
+        <v>5</v>
+      </c>
+      <c r="C10" s="7">
+        <v>20</v>
+      </c>
+      <c r="D10" s="7">
+        <v>0</v>
+      </c>
+      <c r="E10" s="7">
+        <v>1</v>
+      </c>
+      <c r="F10" s="15">
+        <v>-0.56299999999999994</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7">
+        <v>20</v>
+      </c>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7">
+        <v>0</v>
+      </c>
+      <c r="F11" s="4">
+        <v>-4.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="13"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="13"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="13"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix bug in match to normalize distance
</commit_message>
<xml_diff>
--- a/Docs/log_debug9Sep2016.xlsx
+++ b/Docs/log_debug9Sep2016.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\projects\sequential_invest\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\projects\sequential_invest\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="18">
   <si>
     <t>k</t>
   </si>
@@ -78,11 +78,14 @@
   <si>
     <t>limited stocks</t>
   </si>
+  <si>
+    <t>S2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -198,15 +201,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -218,6 +212,15 @@
     </xf>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -590,16 +593,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>400051</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>36635</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>117231</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>495301</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>80311</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>212482</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>52811</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -616,8 +619,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5276851" y="3429000"/>
-          <a:ext cx="4972050" cy="3128311"/>
+          <a:off x="5509847" y="3736731"/>
+          <a:ext cx="3824654" cy="2412080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -631,13 +634,13 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>556847</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>582492</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>175165</xdr:rowOff>
+      <xdr:colOff>161193</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>104125</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -654,8 +657,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5421924" y="0"/>
-          <a:ext cx="5498856" cy="3413665"/>
+          <a:off x="5421924" y="1"/>
+          <a:ext cx="5077557" cy="3152124"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -846,6 +849,44 @@
         <a:xfrm>
           <a:off x="20588654" y="3209193"/>
           <a:ext cx="4535365" cy="3014442"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>249117</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>117231</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>287165</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>78217</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9371136" y="3736731"/>
+          <a:ext cx="4294991" cy="2437486"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1157,7 +1198,7 @@
   <dimension ref="A1:Q33"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1200,10 +1241,10 @@
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="14">
         <v>10</v>
       </c>
       <c r="C2" s="3">
@@ -1230,8 +1271,8 @@
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
-      <c r="B3" s="10"/>
+      <c r="A3" s="15"/>
+      <c r="B3" s="15"/>
       <c r="C3" s="3">
         <v>0</v>
       </c>
@@ -1256,8 +1297,8 @@
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
-      <c r="B4" s="10"/>
+      <c r="A4" s="15"/>
+      <c r="B4" s="15"/>
       <c r="C4" s="3">
         <v>20</v>
       </c>
@@ -1282,8 +1323,8 @@
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="B5" s="11"/>
+      <c r="A5" s="15"/>
+      <c r="B5" s="16"/>
       <c r="C5" s="3">
         <v>20</v>
       </c>
@@ -1308,8 +1349,8 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
-      <c r="B6" s="9">
+      <c r="A6" s="15"/>
+      <c r="B6" s="14">
         <v>5</v>
       </c>
       <c r="C6" s="3">
@@ -1336,8 +1377,8 @@
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
+      <c r="A7" s="15"/>
+      <c r="B7" s="15"/>
       <c r="C7" s="3">
         <v>0</v>
       </c>
@@ -1362,8 +1403,8 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
+      <c r="A8" s="15"/>
+      <c r="B8" s="15"/>
       <c r="C8" s="3">
         <v>20</v>
       </c>
@@ -1388,8 +1429,8 @@
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
-      <c r="B9" s="11"/>
+      <c r="A9" s="15"/>
+      <c r="B9" s="16"/>
       <c r="C9" s="3">
         <v>20</v>
       </c>
@@ -1414,8 +1455,8 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
-      <c r="B10" s="9" t="s">
+      <c r="A10" s="15"/>
+      <c r="B10" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="3">
@@ -1442,8 +1483,8 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10"/>
+      <c r="A11" s="15"/>
+      <c r="B11" s="15"/>
       <c r="C11" s="3">
         <v>0</v>
       </c>
@@ -1468,8 +1509,8 @@
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
+      <c r="A12" s="15"/>
+      <c r="B12" s="15"/>
       <c r="C12" s="3">
         <v>20</v>
       </c>
@@ -1494,8 +1535,8 @@
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
-      <c r="B13" s="11"/>
+      <c r="A13" s="15"/>
+      <c r="B13" s="16"/>
       <c r="C13" s="3">
         <v>20</v>
       </c>
@@ -1520,8 +1561,8 @@
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
-      <c r="B14" s="9" t="s">
+      <c r="A14" s="15"/>
+      <c r="B14" s="14" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="3">
@@ -1548,8 +1589,8 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="10"/>
-      <c r="B15" s="10"/>
+      <c r="A15" s="15"/>
+      <c r="B15" s="15"/>
       <c r="C15" s="3">
         <v>0</v>
       </c>
@@ -1574,8 +1615,8 @@
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
-      <c r="B16" s="10"/>
+      <c r="A16" s="15"/>
+      <c r="B16" s="15"/>
       <c r="C16" s="3">
         <v>20</v>
       </c>
@@ -1600,8 +1641,8 @@
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
-      <c r="B17" s="11"/>
+      <c r="A17" s="16"/>
+      <c r="B17" s="16"/>
       <c r="C17" s="3">
         <v>20</v>
       </c>
@@ -1626,10 +1667,10 @@
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="14" t="s">
         <v>7</v>
       </c>
       <c r="C18" s="3">
@@ -1661,8 +1702,8 @@
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
-      <c r="B19" s="10"/>
+      <c r="A19" s="15"/>
+      <c r="B19" s="15"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="2"/>
@@ -1679,8 +1720,8 @@
       <c r="P19" s="2"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
-      <c r="B20" s="10"/>
+      <c r="A20" s="15"/>
+      <c r="B20" s="15"/>
       <c r="C20" s="3">
         <v>20</v>
       </c>
@@ -1706,8 +1747,8 @@
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21" s="10"/>
-      <c r="B21" s="10"/>
+      <c r="A21" s="15"/>
+      <c r="B21" s="15"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="2"/>
@@ -1724,8 +1765,8 @@
       <c r="P21" s="2"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A22" s="10"/>
-      <c r="B22" s="10"/>
+      <c r="A22" s="15"/>
+      <c r="B22" s="15"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="2"/>
@@ -1742,8 +1783,8 @@
       <c r="P22" s="2"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A23" s="10"/>
-      <c r="B23" s="10"/>
+      <c r="A23" s="15"/>
+      <c r="B23" s="15"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="2"/>
@@ -1760,8 +1801,8 @@
       <c r="P23" s="2"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" s="10"/>
-      <c r="B24" s="10"/>
+      <c r="A24" s="15"/>
+      <c r="B24" s="15"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="2"/>
@@ -1778,8 +1819,8 @@
       <c r="P24" s="2"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A25" s="10"/>
-      <c r="B25" s="10"/>
+      <c r="A25" s="15"/>
+      <c r="B25" s="15"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="2"/>
@@ -1796,8 +1837,8 @@
       <c r="P25" s="2"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A26" s="10"/>
-      <c r="B26" s="10"/>
+      <c r="A26" s="15"/>
+      <c r="B26" s="15"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="2"/>
@@ -1814,8 +1855,8 @@
       <c r="P26" s="2"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A27" s="10"/>
-      <c r="B27" s="10"/>
+      <c r="A27" s="15"/>
+      <c r="B27" s="15"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="2"/>
@@ -1832,8 +1873,8 @@
       <c r="P27" s="2"/>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A28" s="10"/>
-      <c r="B28" s="10"/>
+      <c r="A28" s="15"/>
+      <c r="B28" s="15"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="2"/>
@@ -1850,8 +1891,8 @@
       <c r="P28" s="2"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A29" s="10"/>
-      <c r="B29" s="10"/>
+      <c r="A29" s="15"/>
+      <c r="B29" s="15"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="2"/>
@@ -1868,8 +1909,8 @@
       <c r="P29" s="2"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A30" s="10"/>
-      <c r="B30" s="10"/>
+      <c r="A30" s="15"/>
+      <c r="B30" s="15"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="2"/>
@@ -1886,8 +1927,8 @@
       <c r="P30" s="2"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A31" s="10"/>
-      <c r="B31" s="10"/>
+      <c r="A31" s="15"/>
+      <c r="B31" s="15"/>
       <c r="C31" s="3">
         <v>0</v>
       </c>
@@ -1917,8 +1958,8 @@
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A32" s="10"/>
-      <c r="B32" s="10"/>
+      <c r="A32" s="15"/>
+      <c r="B32" s="15"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="2"/>
@@ -1935,8 +1976,8 @@
       <c r="P32" s="2"/>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A33" s="11"/>
-      <c r="B33" s="11"/>
+      <c r="A33" s="16"/>
+      <c r="B33" s="16"/>
       <c r="C33" s="3">
         <v>20</v>
       </c>
@@ -1980,8 +2021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="AD1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AQ30" sqref="AQ30"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="O35" sqref="O35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1996,7 +2037,7 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2094,23 +2135,23 @@
       <c r="B6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="9">
         <v>20</v>
       </c>
       <c r="D6" s="7">
         <v>0</v>
       </c>
-      <c r="E6" s="14">
+      <c r="E6" s="11">
         <v>1</v>
       </c>
-      <c r="F6" s="16">
+      <c r="F6" s="13">
         <v>0.47299999999999998</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="7"/>
-      <c r="C7" s="14">
+      <c r="C7" s="11">
         <v>20</v>
       </c>
       <c r="D7" s="7"/>
@@ -2151,7 +2192,7 @@
       <c r="E10" s="7">
         <v>1</v>
       </c>
-      <c r="F10" s="15">
+      <c r="F10" s="12">
         <v>-0.56299999999999994</v>
       </c>
     </row>
@@ -2186,94 +2227,136 @@
       <c r="F13" s="2"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
+      <c r="A14" s="2"/>
+      <c r="B14" s="7">
+        <v>10</v>
+      </c>
+      <c r="C14" s="7">
+        <v>0</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="7">
+        <v>0</v>
+      </c>
+      <c r="F14" s="4">
+        <v>-0.32600000000000001</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
+      <c r="A15" s="2"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7">
+        <v>0</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="7">
+        <v>1</v>
+      </c>
+      <c r="F15" s="4">
+        <v>-0.30599999999999999</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="13"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="13"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="13"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="13"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="13"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
+      <c r="A16" s="2"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7">
+        <v>20</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="7">
+        <v>0</v>
+      </c>
+      <c r="F16" s="4">
+        <v>-0.76600000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7">
+        <v>20</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="7">
+        <v>1</v>
+      </c>
+      <c r="F17" s="4">
+        <v>-0.72799999999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>